<commit_message>
added a few things to word
</commit_message>
<xml_diff>
--- a/DataPreparation_BarChart.xlsx
+++ b/DataPreparation_BarChart.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebraeckow\Desktop\Gatech\ISYE6740 Computational Data Analytics\Project_Code\isye6740-project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksmit2\Desktop\PP\Masters\GA_TECH_6470\Projects\isye6740-project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F019FF48-36A3-4D48-9593-712F23C68F15}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D3E0E16-9B49-4A48-8D8F-22188B55ED8C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{439F9D31-767D-4C1C-B3E0-BE621A230FC3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{439F9D31-767D-4C1C-B3E0-BE621A230FC3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -205,13 +205,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.72</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.72</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.71</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -684,7 +684,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.72</c:v>
+                  <c:v>0.65</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.59499999999999997</c:v>
@@ -749,7 +749,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.72</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.626</c:v>
@@ -814,7 +814,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>0.71</c:v>
+                  <c:v>0.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.67600000000000005</c:v>
@@ -2161,15 +2161,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>861060</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>167640</xdr:rowOff>
+      <xdr:colOff>975360</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>154940</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>487680</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:colOff>601980</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>124460</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2496,19 +2496,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76D98FF-4A07-4DBE-8A35-36387A6883B0}">
   <dimension ref="G6:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="E16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="7" max="7" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.33203125" customWidth="1"/>
-    <col min="10" max="10" width="35.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.36328125" customWidth="1"/>
+    <col min="10" max="10" width="35.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="7:10" x14ac:dyDescent="0.35">
       <c r="H6" s="1" t="s">
         <v>3</v>
       </c>
@@ -2519,21 +2519,21 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G7" s="1" t="s">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="I7">
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="J7">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
     </row>
-    <row r="8" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G8" s="1" t="s">
         <v>1</v>
       </c>
@@ -2547,7 +2547,7 @@
         <v>0.67600000000000005</v>
       </c>
     </row>
-    <row r="9" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>0.71709999999999996</v>
       </c>
     </row>
-    <row r="13" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="7:10" x14ac:dyDescent="0.35">
       <c r="H13" s="1" t="s">
         <v>0</v>
       </c>
@@ -2572,12 +2572,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="H14">
-        <v>0.72</v>
+        <v>0.65</v>
       </c>
       <c r="I14">
         <v>0.59499999999999997</v>
@@ -2586,12 +2586,12 @@
         <v>0.66</v>
       </c>
     </row>
-    <row r="15" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G15" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H15">
-        <v>0.72</v>
+        <v>0.61</v>
       </c>
       <c r="I15">
         <v>0.626</v>
@@ -2600,12 +2600,12 @@
         <v>0.69689999999999996</v>
       </c>
     </row>
-    <row r="16" spans="7:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="7:10" x14ac:dyDescent="0.35">
       <c r="G16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="H16">
-        <v>0.71</v>
+        <v>0.7</v>
       </c>
       <c r="I16">
         <v>0.67600000000000005</v>

</xml_diff>